<commit_message>
WORKING CODE FOR NEW STUDENT
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\holdb\Documents\CPSC-481-Project-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96495E40-11B8-41CF-AC31-5BA517401ACF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F328EA81-E02E-49B7-8DCE-781201EA2F8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2205" yWindow="2205" windowWidth="21600" windowHeight="11295" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -200,9 +200,6 @@
     <t>Math Structures 2</t>
   </si>
   <si>
-    <t xml:space="preserve">MATH 338 </t>
-  </si>
-  <si>
     <t>Statistics Applied to Natural Sciences</t>
   </si>
   <si>
@@ -318,6 +315,9 @@
   </si>
   <si>
     <t>Graduation Requirement</t>
+  </si>
+  <si>
+    <t>MATH 338</t>
   </si>
 </sst>
 </file>
@@ -764,8 +764,8 @@
   <dimension ref="A1:AA52"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A34" sqref="A34"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.7109375" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1308,7 +1308,7 @@
         <v>45</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>54</v>
+        <v>93</v>
       </c>
       <c r="C22" s="3">
         <v>4</v>
@@ -1324,15 +1324,15 @@
         <v>4</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="B23" s="3" t="s">
-        <v>57</v>
       </c>
       <c r="C23" s="3">
         <v>3</v>
@@ -1348,15 +1348,15 @@
         <v>6</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C24" s="3">
         <v>3</v>
@@ -1372,15 +1372,15 @@
         <v>6</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C25" s="3">
         <v>3</v>
@@ -1396,15 +1396,15 @@
         <v>6</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="3">
         <v>3</v>
@@ -1420,15 +1420,15 @@
         <v>6</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C27" s="3">
         <v>3</v>
@@ -1444,15 +1444,15 @@
         <v>6</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" s="3" t="s">
         <v>67</v>
-      </c>
-      <c r="B28" s="3" t="s">
-        <v>68</v>
       </c>
       <c r="C28" s="3">
         <v>3</v>
@@ -1468,15 +1468,15 @@
         <v>7</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C29" s="3">
         <v>3</v>
@@ -1492,15 +1492,15 @@
         <v>7</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C30" s="3">
         <v>3</v>
@@ -1516,15 +1516,15 @@
         <v>7</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C31" s="3">
         <v>3</v>
@@ -1540,15 +1540,15 @@
         <v>7</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A32" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C32" s="3">
         <v>3</v>
@@ -1564,15 +1564,15 @@
         <v>7</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A33" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C33" s="3">
         <v>3</v>
@@ -1588,15 +1588,15 @@
         <v>7</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A34" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C34" s="3">
         <v>3</v>
@@ -1612,15 +1612,15 @@
         <v>7</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A35" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C35" s="3">
         <v>3</v>
@@ -1636,15 +1636,15 @@
         <v>7</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A36" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="B36" s="3" t="s">
-        <v>85</v>
       </c>
       <c r="C36" s="3">
         <v>3</v>
@@ -1660,15 +1660,15 @@
         <v>7</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A37" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C37" s="3">
         <v>3</v>
@@ -1684,15 +1684,15 @@
         <v>7</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C38" s="3">
         <v>3</v>
@@ -1708,15 +1708,15 @@
         <v>7</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">
       <c r="A39" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C39" s="3">
         <v>3</v>
@@ -1732,7 +1732,7 @@
         <v>7</v>
       </c>
       <c r="G39" s="2" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="14.25" x14ac:dyDescent="0.2">

</xml_diff>